<commit_message>
mise à jour capteur
</commit_message>
<xml_diff>
--- a/Liste commande V1 (2).xlsx
+++ b/Liste commande V1 (2).xlsx
@@ -8,35 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\k.lancereau\Desktop\LoRa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E91069A2-8904-4E0E-ACEC-A468985CC671}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C243AF7B-5B43-4DB7-B127-79E347E5EF7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C425252E-849C-43A2-9406-B174143CEA98}"/>
   </bookViews>
   <sheets>
     <sheet name="Fonction envoyée au node" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>X</t>
   </si>
@@ -71,6 +60,12 @@
   </si>
   <si>
     <t>Fonction</t>
+  </si>
+  <si>
+    <t>mise en service d'une gateway neuve</t>
+  </si>
+  <si>
+    <t>eviter reset intempestif</t>
   </si>
 </sst>
 </file>
@@ -455,15 +450,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCD0F4F5-A544-40A2-AE41-B1F7DBDB1EB8}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" customWidth="1"/>
+    <col min="1" max="1" width="34.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="130" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -512,6 +507,14 @@
         <v>0</v>
       </c>
     </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update Liste commande V1 (2).xlsx
</commit_message>
<xml_diff>
--- a/Liste commande V1 (2).xlsx
+++ b/Liste commande V1 (2).xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\k.lancereau\Desktop\LoRa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C243AF7B-5B43-4DB7-B127-79E347E5EF7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6602B656-0C81-46A2-B98C-D15E6B75C93F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C425252E-849C-43A2-9406-B174143CEA98}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{C425252E-849C-43A2-9406-B174143CEA98}"/>
   </bookViews>
   <sheets>
     <sheet name="Fonction envoyée au node" sheetId="1" r:id="rId1"/>
+    <sheet name="Type" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="124">
   <si>
     <t>X</t>
   </si>
@@ -66,13 +67,346 @@
   </si>
   <si>
     <t>eviter reset intempestif</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>07</t>
+  </si>
+  <si>
+    <t>08</t>
+  </si>
+  <si>
+    <t>09</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>capteur</t>
+  </si>
+  <si>
+    <t>actionneur</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>53</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>56</t>
+  </si>
+  <si>
+    <t>57</t>
+  </si>
+  <si>
+    <t>58</t>
+  </si>
+  <si>
+    <t>59</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>61</t>
+  </si>
+  <si>
+    <t>62</t>
+  </si>
+  <si>
+    <t>63</t>
+  </si>
+  <si>
+    <t>64</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>66</t>
+  </si>
+  <si>
+    <t>67</t>
+  </si>
+  <si>
+    <t>68</t>
+  </si>
+  <si>
+    <t>69</t>
+  </si>
+  <si>
+    <t>70</t>
+  </si>
+  <si>
+    <t>71</t>
+  </si>
+  <si>
+    <t>72</t>
+  </si>
+  <si>
+    <t>73</t>
+  </si>
+  <si>
+    <t>74</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>76</t>
+  </si>
+  <si>
+    <t>77</t>
+  </si>
+  <si>
+    <t>78</t>
+  </si>
+  <si>
+    <t>79</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>81</t>
+  </si>
+  <si>
+    <t>82</t>
+  </si>
+  <si>
+    <t>83</t>
+  </si>
+  <si>
+    <t>84</t>
+  </si>
+  <si>
+    <t>85</t>
+  </si>
+  <si>
+    <t>86</t>
+  </si>
+  <si>
+    <t>87</t>
+  </si>
+  <si>
+    <t>88</t>
+  </si>
+  <si>
+    <t>89</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>91</t>
+  </si>
+  <si>
+    <t>92</t>
+  </si>
+  <si>
+    <t>93</t>
+  </si>
+  <si>
+    <t>94</t>
+  </si>
+  <si>
+    <t>95</t>
+  </si>
+  <si>
+    <t>96</t>
+  </si>
+  <si>
+    <t>97</t>
+  </si>
+  <si>
+    <t>98</t>
+  </si>
+  <si>
+    <t>99</t>
+  </si>
+  <si>
+    <t>binaire</t>
+  </si>
+  <si>
+    <t>numérique</t>
+  </si>
+  <si>
+    <t>descriptif</t>
+  </si>
+  <si>
+    <t>capteur simple tout ou rien 1 byte</t>
+  </si>
+  <si>
+    <t>base</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Atmega168Pa equivalent arduino nano minicore </t>
+  </si>
+  <si>
+    <t>00</t>
+  </si>
+  <si>
+    <t>passerelle LoRa &lt;=&gt; Mqtt</t>
+  </si>
+  <si>
+    <t>ttgo LoRa ESP32</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -88,16 +422,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -105,11 +451,43 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="1" diagonalDown="1">
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal style="thin">
+        <color indexed="64"/>
+      </diagonal>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -132,6 +510,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -452,7 +833,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCD0F4F5-A544-40A2-AE41-B1F7DBDB1EB8}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -519,4 +900,1155 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A150C31-50B7-4C4C-A00A-295F065703B3}">
+  <dimension ref="A1:G101"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="44.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="10"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B35" s="8"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="8"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B39" s="8"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B41" s="8"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B42" s="8"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B43" s="8"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B44" s="8"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="8"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B45" s="8"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="8"/>
+      <c r="E45" s="8"/>
+      <c r="F45" s="8"/>
+      <c r="G45" s="8"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B46" s="8"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="8"/>
+      <c r="E46" s="8"/>
+      <c r="F46" s="8"/>
+      <c r="G46" s="8"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B47" s="8"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="8"/>
+      <c r="E47" s="8"/>
+      <c r="F47" s="8"/>
+      <c r="G47" s="8"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B48" s="8"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="8"/>
+      <c r="E48" s="8"/>
+      <c r="F48" s="8"/>
+      <c r="G48" s="8"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B49" s="8"/>
+      <c r="C49" s="8"/>
+      <c r="D49" s="8"/>
+      <c r="E49" s="8"/>
+      <c r="F49" s="8"/>
+      <c r="G49" s="8"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B50" s="8"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="8"/>
+      <c r="E50" s="8"/>
+      <c r="F50" s="8"/>
+      <c r="G50" s="8"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B51" s="8"/>
+      <c r="C51" s="8"/>
+      <c r="D51" s="8"/>
+      <c r="E51" s="8"/>
+      <c r="F51" s="8"/>
+      <c r="G51" s="8"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B52" s="8"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="8"/>
+      <c r="E52" s="8"/>
+      <c r="F52" s="8"/>
+      <c r="G52" s="8"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B53" s="8"/>
+      <c r="C53" s="8"/>
+      <c r="D53" s="8"/>
+      <c r="E53" s="8"/>
+      <c r="F53" s="8"/>
+      <c r="G53" s="8"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B54" s="8"/>
+      <c r="C54" s="8"/>
+      <c r="D54" s="8"/>
+      <c r="E54" s="8"/>
+      <c r="F54" s="8"/>
+      <c r="G54" s="8"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B55" s="8"/>
+      <c r="C55" s="8"/>
+      <c r="D55" s="8"/>
+      <c r="E55" s="8"/>
+      <c r="F55" s="8"/>
+      <c r="G55" s="8"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B56" s="8"/>
+      <c r="C56" s="8"/>
+      <c r="D56" s="8"/>
+      <c r="E56" s="8"/>
+      <c r="F56" s="8"/>
+      <c r="G56" s="8"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B57" s="8"/>
+      <c r="C57" s="8"/>
+      <c r="D57" s="8"/>
+      <c r="E57" s="8"/>
+      <c r="F57" s="8"/>
+      <c r="G57" s="8"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B58" s="8"/>
+      <c r="C58" s="8"/>
+      <c r="D58" s="8"/>
+      <c r="E58" s="8"/>
+      <c r="F58" s="8"/>
+      <c r="G58" s="8"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B59" s="8"/>
+      <c r="C59" s="8"/>
+      <c r="D59" s="8"/>
+      <c r="E59" s="8"/>
+      <c r="F59" s="8"/>
+      <c r="G59" s="8"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B60" s="8"/>
+      <c r="C60" s="8"/>
+      <c r="D60" s="8"/>
+      <c r="E60" s="8"/>
+      <c r="F60" s="8"/>
+      <c r="G60" s="8"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B61" s="8"/>
+      <c r="C61" s="8"/>
+      <c r="D61" s="8"/>
+      <c r="E61" s="8"/>
+      <c r="F61" s="8"/>
+      <c r="G61" s="8"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B62" s="8"/>
+      <c r="C62" s="8"/>
+      <c r="D62" s="8"/>
+      <c r="E62" s="8"/>
+      <c r="F62" s="8"/>
+      <c r="G62" s="8"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B63" s="8"/>
+      <c r="C63" s="8"/>
+      <c r="D63" s="8"/>
+      <c r="E63" s="8"/>
+      <c r="F63" s="8"/>
+      <c r="G63" s="8"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B64" s="8"/>
+      <c r="C64" s="8"/>
+      <c r="D64" s="8"/>
+      <c r="E64" s="8"/>
+      <c r="F64" s="8"/>
+      <c r="G64" s="8"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B65" s="8"/>
+      <c r="C65" s="8"/>
+      <c r="D65" s="8"/>
+      <c r="E65" s="8"/>
+      <c r="F65" s="8"/>
+      <c r="G65" s="8"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B66" s="8"/>
+      <c r="C66" s="8"/>
+      <c r="D66" s="8"/>
+      <c r="E66" s="8"/>
+      <c r="F66" s="8"/>
+      <c r="G66" s="8"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B67" s="8"/>
+      <c r="C67" s="8"/>
+      <c r="D67" s="8"/>
+      <c r="E67" s="8"/>
+      <c r="F67" s="8"/>
+      <c r="G67" s="8"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B68" s="8"/>
+      <c r="C68" s="8"/>
+      <c r="D68" s="8"/>
+      <c r="E68" s="8"/>
+      <c r="F68" s="8"/>
+      <c r="G68" s="8"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B69" s="8"/>
+      <c r="C69" s="8"/>
+      <c r="D69" s="8"/>
+      <c r="E69" s="8"/>
+      <c r="F69" s="8"/>
+      <c r="G69" s="8"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="B70" s="8"/>
+      <c r="C70" s="8"/>
+      <c r="D70" s="8"/>
+      <c r="E70" s="8"/>
+      <c r="F70" s="8"/>
+      <c r="G70" s="8"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B71" s="8"/>
+      <c r="C71" s="8"/>
+      <c r="D71" s="8"/>
+      <c r="E71" s="8"/>
+      <c r="F71" s="8"/>
+      <c r="G71" s="8"/>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B72" s="8"/>
+      <c r="C72" s="8"/>
+      <c r="D72" s="8"/>
+      <c r="E72" s="8"/>
+      <c r="F72" s="8"/>
+      <c r="G72" s="8"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B73" s="8"/>
+      <c r="C73" s="8"/>
+      <c r="D73" s="8"/>
+      <c r="E73" s="8"/>
+      <c r="F73" s="8"/>
+      <c r="G73" s="8"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B74" s="8"/>
+      <c r="C74" s="8"/>
+      <c r="D74" s="8"/>
+      <c r="E74" s="8"/>
+      <c r="F74" s="8"/>
+      <c r="G74" s="8"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B75" s="8"/>
+      <c r="C75" s="8"/>
+      <c r="D75" s="8"/>
+      <c r="E75" s="8"/>
+      <c r="F75" s="8"/>
+      <c r="G75" s="8"/>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="B76" s="8"/>
+      <c r="C76" s="8"/>
+      <c r="D76" s="8"/>
+      <c r="E76" s="8"/>
+      <c r="F76" s="8"/>
+      <c r="G76" s="8"/>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="B77" s="8"/>
+      <c r="C77" s="8"/>
+      <c r="D77" s="8"/>
+      <c r="E77" s="8"/>
+      <c r="F77" s="8"/>
+      <c r="G77" s="8"/>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="B78" s="8"/>
+      <c r="C78" s="8"/>
+      <c r="D78" s="8"/>
+      <c r="E78" s="8"/>
+      <c r="F78" s="8"/>
+      <c r="G78" s="8"/>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="B79" s="8"/>
+      <c r="C79" s="8"/>
+      <c r="D79" s="8"/>
+      <c r="E79" s="8"/>
+      <c r="F79" s="8"/>
+      <c r="G79" s="8"/>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B80" s="8"/>
+      <c r="C80" s="8"/>
+      <c r="D80" s="8"/>
+      <c r="E80" s="8"/>
+      <c r="F80" s="8"/>
+      <c r="G80" s="8"/>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="B81" s="8"/>
+      <c r="C81" s="8"/>
+      <c r="D81" s="8"/>
+      <c r="E81" s="8"/>
+      <c r="F81" s="8"/>
+      <c r="G81" s="8"/>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B82" s="8"/>
+      <c r="C82" s="8"/>
+      <c r="D82" s="8"/>
+      <c r="E82" s="8"/>
+      <c r="F82" s="8"/>
+      <c r="G82" s="8"/>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="B83" s="8"/>
+      <c r="C83" s="8"/>
+      <c r="D83" s="8"/>
+      <c r="E83" s="8"/>
+      <c r="F83" s="8"/>
+      <c r="G83" s="8"/>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B84" s="8"/>
+      <c r="C84" s="8"/>
+      <c r="D84" s="8"/>
+      <c r="E84" s="8"/>
+      <c r="F84" s="8"/>
+      <c r="G84" s="8"/>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="B85" s="8"/>
+      <c r="C85" s="8"/>
+      <c r="D85" s="8"/>
+      <c r="E85" s="8"/>
+      <c r="F85" s="8"/>
+      <c r="G85" s="8"/>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="B86" s="8"/>
+      <c r="C86" s="8"/>
+      <c r="D86" s="8"/>
+      <c r="E86" s="8"/>
+      <c r="F86" s="8"/>
+      <c r="G86" s="8"/>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B87" s="8"/>
+      <c r="C87" s="8"/>
+      <c r="D87" s="8"/>
+      <c r="E87" s="8"/>
+      <c r="F87" s="8"/>
+      <c r="G87" s="8"/>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="B88" s="8"/>
+      <c r="C88" s="8"/>
+      <c r="D88" s="8"/>
+      <c r="E88" s="8"/>
+      <c r="F88" s="8"/>
+      <c r="G88" s="8"/>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="B89" s="8"/>
+      <c r="C89" s="8"/>
+      <c r="D89" s="8"/>
+      <c r="E89" s="8"/>
+      <c r="F89" s="8"/>
+      <c r="G89" s="8"/>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B90" s="8"/>
+      <c r="C90" s="8"/>
+      <c r="D90" s="8"/>
+      <c r="E90" s="8"/>
+      <c r="F90" s="8"/>
+      <c r="G90" s="8"/>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="B91" s="8"/>
+      <c r="C91" s="8"/>
+      <c r="D91" s="8"/>
+      <c r="E91" s="8"/>
+      <c r="F91" s="8"/>
+      <c r="G91" s="8"/>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B92" s="8"/>
+      <c r="C92" s="8"/>
+      <c r="D92" s="8"/>
+      <c r="E92" s="8"/>
+      <c r="F92" s="8"/>
+      <c r="G92" s="8"/>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="B93" s="8"/>
+      <c r="C93" s="8"/>
+      <c r="D93" s="8"/>
+      <c r="E93" s="8"/>
+      <c r="F93" s="8"/>
+      <c r="G93" s="8"/>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="B94" s="8"/>
+      <c r="C94" s="8"/>
+      <c r="D94" s="8"/>
+      <c r="E94" s="8"/>
+      <c r="F94" s="8"/>
+      <c r="G94" s="8"/>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B95" s="8"/>
+      <c r="C95" s="8"/>
+      <c r="D95" s="8"/>
+      <c r="E95" s="8"/>
+      <c r="F95" s="8"/>
+      <c r="G95" s="8"/>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B96" s="8"/>
+      <c r="C96" s="8"/>
+      <c r="D96" s="8"/>
+      <c r="E96" s="8"/>
+      <c r="F96" s="8"/>
+      <c r="G96" s="8"/>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A97" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="B97" s="8"/>
+      <c r="C97" s="8"/>
+      <c r="D97" s="8"/>
+      <c r="E97" s="8"/>
+      <c r="F97" s="8"/>
+      <c r="G97" s="8"/>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B98" s="8"/>
+      <c r="C98" s="8"/>
+      <c r="D98" s="8"/>
+      <c r="E98" s="8"/>
+      <c r="F98" s="8"/>
+      <c r="G98" s="8"/>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="B99" s="8"/>
+      <c r="C99" s="8"/>
+      <c r="D99" s="8"/>
+      <c r="E99" s="8"/>
+      <c r="F99" s="8"/>
+      <c r="G99" s="8"/>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="B100" s="8"/>
+      <c r="C100" s="8"/>
+      <c r="D100" s="8"/>
+      <c r="E100" s="8"/>
+      <c r="F100" s="8"/>
+      <c r="G100" s="8"/>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B101" s="8"/>
+      <c r="C101" s="8"/>
+      <c r="D101" s="8"/>
+      <c r="E101" s="8"/>
+      <c r="F101" s="8"/>
+      <c r="G101" s="8"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>